<commit_message>
Werkend insert script & db aanpassingen
</commit_message>
<xml_diff>
--- a/insert_script/data/pizza_ingredienten.xlsx
+++ b/insert_script/data/pizza_ingredienten.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10909"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Onderwijs\Ontwikkeling\OvP S4 nj2017\Casus\Mario data\voor studenten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nils.van.eijk/Documents/School/Mario/insert_script/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FF8E59-946B-2C4B-80D8-6AF552FCC45C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11040"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -315,11 +316,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;€&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,7 +360,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -658,26 +659,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="108" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -716,7 +719,7 @@
       </c>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -745,7 +748,7 @@
         <v>95</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K2" t="s">
         <v>16</v>
@@ -754,7 +757,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -783,7 +786,7 @@
         <v>95</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K3" t="s">
         <v>18</v>
@@ -792,7 +795,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -830,7 +833,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -868,7 +871,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -906,7 +909,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -944,7 +947,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -982,7 +985,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1020,7 +1023,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1058,7 +1061,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1096,7 +1099,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1172,7 +1175,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1210,7 +1213,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1248,7 +1251,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1286,7 +1289,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1324,7 +1327,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1362,7 +1365,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1400,7 +1403,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1438,7 +1441,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1476,7 +1479,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1514,7 +1517,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1552,7 +1555,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1590,7 +1593,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1628,7 +1631,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -1666,7 +1669,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1704,7 +1707,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -1742,7 +1745,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -1780,7 +1783,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -1818,7 +1821,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -1856,7 +1859,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -1894,7 +1897,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -1932,7 +1935,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1970,7 +1973,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -2008,7 +2011,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -2046,7 +2049,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -2084,7 +2087,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -2122,7 +2125,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -2160,7 +2163,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -2198,7 +2201,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -2236,7 +2239,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -2274,7 +2277,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -2312,7 +2315,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -2350,7 +2353,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -2388,7 +2391,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -2426,7 +2429,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -2464,7 +2467,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -2502,7 +2505,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -2540,7 +2543,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -2578,7 +2581,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -2616,7 +2619,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -2654,7 +2657,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -2692,7 +2695,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -2730,7 +2733,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -2768,7 +2771,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -2806,7 +2809,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -2844,7 +2847,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12">
       <c r="A58" t="s">
         <v>12</v>
       </c>
@@ -2882,7 +2885,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12">
       <c r="A59" t="s">
         <v>12</v>
       </c>
@@ -2920,7 +2923,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12">
       <c r="A60" t="s">
         <v>12</v>
       </c>
@@ -2958,7 +2961,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -2996,7 +2999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -3034,7 +3037,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12">
       <c r="A63" t="s">
         <v>12</v>
       </c>
@@ -3072,7 +3075,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -3110,7 +3113,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12">
       <c r="A65" t="s">
         <v>12</v>
       </c>
@@ -3148,7 +3151,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -3186,7 +3189,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12">
       <c r="A67" t="s">
         <v>12</v>
       </c>
@@ -3224,7 +3227,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -3262,7 +3265,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12">
       <c r="A69" t="s">
         <v>12</v>
       </c>
@@ -3300,7 +3303,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12">
       <c r="A70" t="s">
         <v>12</v>
       </c>
@@ -3338,7 +3341,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12">
       <c r="A71" t="s">
         <v>12</v>
       </c>
@@ -3376,7 +3379,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12">
       <c r="A72" t="s">
         <v>12</v>
       </c>
@@ -3414,7 +3417,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12">
       <c r="A73" t="s">
         <v>12</v>
       </c>
@@ -3452,7 +3455,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12">
       <c r="A74" t="s">
         <v>12</v>
       </c>
@@ -3490,7 +3493,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12">
       <c r="A75" t="s">
         <v>12</v>
       </c>
@@ -3528,7 +3531,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12">
       <c r="A76" t="s">
         <v>12</v>
       </c>
@@ -3566,7 +3569,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12">
       <c r="A77" t="s">
         <v>12</v>
       </c>
@@ -3604,7 +3607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12">
       <c r="A78" t="s">
         <v>12</v>
       </c>
@@ -3642,7 +3645,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12">
       <c r="A79" t="s">
         <v>12</v>
       </c>
@@ -3680,7 +3683,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12">
       <c r="A80" t="s">
         <v>12</v>
       </c>
@@ -3718,7 +3721,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12">
       <c r="A81" t="s">
         <v>12</v>
       </c>
@@ -3756,7 +3759,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12">
       <c r="A82" t="s">
         <v>12</v>
       </c>
@@ -3794,7 +3797,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12">
       <c r="A83" t="s">
         <v>12</v>
       </c>
@@ -3832,7 +3835,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12">
       <c r="A84" t="s">
         <v>12</v>
       </c>
@@ -3870,7 +3873,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12">
       <c r="A85" t="s">
         <v>12</v>
       </c>
@@ -3908,7 +3911,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12">
       <c r="A86" t="s">
         <v>12</v>
       </c>
@@ -3946,7 +3949,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12">
       <c r="A87" t="s">
         <v>12</v>
       </c>
@@ -3984,7 +3987,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12">
       <c r="A88" t="s">
         <v>12</v>
       </c>
@@ -4022,7 +4025,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12">
       <c r="A89" t="s">
         <v>12</v>
       </c>
@@ -4060,7 +4063,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12">
       <c r="A90" t="s">
         <v>12</v>
       </c>
@@ -4098,7 +4101,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12">
       <c r="A91" t="s">
         <v>12</v>
       </c>
@@ -4136,7 +4139,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12">
       <c r="A92" t="s">
         <v>12</v>
       </c>
@@ -4174,7 +4177,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12">
       <c r="A93" t="s">
         <v>12</v>
       </c>
@@ -4212,7 +4215,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12">
       <c r="A94" t="s">
         <v>12</v>
       </c>
@@ -4250,7 +4253,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12">
       <c r="A95" t="s">
         <v>12</v>
       </c>
@@ -4288,7 +4291,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12">
       <c r="A96" t="s">
         <v>12</v>
       </c>
@@ -4326,7 +4329,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12">
       <c r="A97" t="s">
         <v>12</v>
       </c>
@@ -4364,7 +4367,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12">
       <c r="A98" t="s">
         <v>12</v>
       </c>
@@ -4402,7 +4405,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12">
       <c r="A99" t="s">
         <v>12</v>
       </c>
@@ -4440,7 +4443,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12">
       <c r="A100" t="s">
         <v>12</v>
       </c>
@@ -4478,7 +4481,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12">
       <c r="A101" t="s">
         <v>12</v>
       </c>
@@ -4516,7 +4519,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12">
       <c r="A102" t="s">
         <v>12</v>
       </c>
@@ -4554,7 +4557,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12">
       <c r="A103" t="s">
         <v>12</v>
       </c>
@@ -4592,7 +4595,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12">
       <c r="A104" t="s">
         <v>12</v>
       </c>
@@ -4630,7 +4633,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12">
       <c r="A105" t="s">
         <v>12</v>
       </c>
@@ -4668,7 +4671,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12">
       <c r="A106" t="s">
         <v>12</v>
       </c>
@@ -4706,7 +4709,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12">
       <c r="A107" t="s">
         <v>12</v>
       </c>
@@ -4744,7 +4747,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12">
       <c r="A108" t="s">
         <v>12</v>
       </c>
@@ -4782,7 +4785,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12">
       <c r="A109" t="s">
         <v>12</v>
       </c>
@@ -4820,7 +4823,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12">
       <c r="A110" t="s">
         <v>12</v>
       </c>
@@ -4858,7 +4861,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12">
       <c r="A111" t="s">
         <v>12</v>
       </c>
@@ -4896,7 +4899,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12">
       <c r="A112" t="s">
         <v>12</v>
       </c>
@@ -4934,7 +4937,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12">
       <c r="A113" t="s">
         <v>12</v>
       </c>
@@ -4972,7 +4975,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12">
       <c r="A114" t="s">
         <v>12</v>
       </c>
@@ -5010,7 +5013,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12">
       <c r="A115" t="s">
         <v>12</v>
       </c>

</xml_diff>